<commit_message>
Update Excel file with latest predictions
</commit_message>
<xml_diff>
--- a/scraper/data/betclever_predictions.xlsx
+++ b/scraper/data/betclever_predictions.xlsx
@@ -475,85 +475,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>27-02-2025 01:30</t>
+          <t>27-02-2025 20:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>MOROCCO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COPA DO NORDESTE</t>
+          <t>BOTOLA PRO</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CSA - Nautico Recife</t>
+          <t>CODM Meknès - Hassania Agadir</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>71.7</v>
+        <v>70</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>2.05</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>27-02-2025 20:00</t>
+          <t>27-02-2025 18:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MOROCCO</t>
+          <t>POLAND</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BOTOLA PRO</t>
+          <t>CUP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CODM Meknès - Hassania Agadir</t>
+          <t>Polonia Warszawa - Puszcza Niepołomice</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>70</v>
       </c>
       <c r="F3" t="n">
-        <v>2.05</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>27-02-2025 18:00</t>
+          <t>28-02-2025 10:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>POLAND</t>
+          <t>AUSTRALIA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CUP</t>
+          <t>NEW SOUTH WALES NPL 2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Polonia Warszawa - Puszcza Niepołomice</t>
+          <t>Blacktown Spartans - Bonnyrigg White Eagles</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>70</v>
+        <v>75.7</v>
       </c>
       <c r="F4" t="n">
-        <v>2.95</v>
+        <v>2.2</v>
       </c>
     </row>
   </sheetData>
@@ -646,7 +646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,82 +689,82 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>27-02-2025 00:30</t>
+          <t>27-02-2025 23:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>WORLD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COPA VERDE</t>
+          <t>CONMEBOL LIBERTADORES</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Manaus FC - Paysandu</t>
+          <t>Cerro Porteno - Monagas SC</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>81.09999999999999</v>
+        <v>84</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>27-02-2025 01:30</t>
+          <t>27-02-2025 18:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>WORLD</t>
+          <t>EGYPT</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CONMEBOL LIBERTADORES</t>
+          <t>PREMIER LEAGUE</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Corinthians - UCV</t>
+          <t>Zamalek SC - Masr</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>76</v>
+        <v>76.7</v>
       </c>
       <c r="F3" t="n">
-        <v>3.5</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>27-02-2025 23:00</t>
+          <t>28-02-2025 21:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>WORLD</t>
+          <t>ENGLAND</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CONMEBOL LIBERTADORES</t>
+          <t>FA CUP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Cerro Porteno - Monagas SC</t>
+          <t>Aston Villa - Cardiff</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>84</v>
+        <v>88.3</v>
       </c>
       <c r="F4" t="n">
         <v>2.1</v>
@@ -773,85 +773,141 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>27-02-2025 01:00</t>
+          <t>01-03-2025 00:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>CHILE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>COPA DO BRASIL</t>
+          <t>PRIMERA DIVISIÓN</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Humaitá - Operario-PR</t>
+          <t>Deportes Limache - Coquimbo Unido</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F5" t="n">
-        <v>2.25</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>27-02-2025 18:00</t>
+          <t>28-02-2025 19:30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EGYPT</t>
+          <t>FRANCE</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PREMIER LEAGUE</t>
+          <t>NATIONAL 1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Zamalek SC - Masr</t>
+          <t>Orleans - Sochaux</t>
         </is>
       </c>
       <c r="E6" t="n">
         <v>76.7</v>
       </c>
       <c r="F6" t="n">
-        <v>2.15</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>27-02-2025 04:05</t>
+          <t>28-02-2025 18:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MEXICO</t>
+          <t>GERMANY</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LIGA MX</t>
+          <t>2. BUNDESLIGA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Atletico San Luis - Guadalajara Chivas</t>
+          <t>FC Schalke 04 - Preußen Münster</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F7" t="n">
-        <v>1.75</v>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IRELAND</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>FIRST DIVISION</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Treaty United - Finn Harps</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ITALY</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SERIE C - GIRONE A</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Giana Erminio - Lumezzane</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>90</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -986,69 +1042,171 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>27-02-2025 04:05</t>
+          <t>28-02-2025 09:35</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MEXICO</t>
+          <t>AUSTRALIA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LIGA MX</t>
+          <t>A-LEAGUE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Atletico San Luis - Guadalajara Chivas</t>
+          <t>Central Coast Mariners - Western United</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F4" t="n">
-        <v>1.95</v>
+        <v>1.62</v>
       </c>
       <c r="G4" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="H4" t="n">
-        <v>3.4</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>27-02-2025 04:30</t>
+          <t>28-02-2025 18:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>WORLD</t>
+          <t>AUSTRIA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CONCACAF CHAMPIONS LEAGUE</t>
+          <t>2. LIGA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Seattle Sounders - Antigua GFC</t>
+          <t>Rapid Wien II - Austria Lustenau</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>66.7</v>
+        <v>85</v>
       </c>
       <c r="F5" t="n">
-        <v>1.53</v>
+        <v>1.77</v>
       </c>
       <c r="G5" t="n">
-        <v>66.7</v>
+        <v>45</v>
       </c>
       <c r="H5" t="n">
-        <v>2.45</v>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Ried - Floridsdorfer AC</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>85</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>40</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CYPRUS</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1. DIVISION</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Anorthosis - Karmiotissa</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G7" t="n">
+        <v>36.3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:20</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GERMANY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>REGIONALLIGA - NORDOST</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>FSV Zwickau - Lokomotive Leipzig</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>75</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G8" t="n">
+        <v>70</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.88</v>
       </c>
     </row>
   </sheetData>
@@ -1062,7 +1220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,69 +1268,69 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>26-02-2025 12:00</t>
+          <t>27-02-2025 21:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TANZANIA</t>
+          <t>ENGLAND</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>LIGI KUU BARA</t>
+          <t>LEAGUE TWO</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Singida Big Stars - Tanzania Prisons</t>
+          <t>Barrow - Carlisle</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F2" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="G2" t="n">
-        <v>0.05</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>27-02-2025 21:00</t>
+          <t>27-02-2025 17:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ENGLAND</t>
+          <t>ALGERIA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LEAGUE TWO</t>
+          <t>LIGUE 1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Barrow - Carlisle</t>
+          <t>JS Saoura - Oued Akbou</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F3" t="n">
         <v>1.8</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.01</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>27-02-2025 17:00</t>
+          <t>27-02-2025 14:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1182,22 +1340,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LIGUE 1</t>
+          <t>LIGUE 2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>JS Saoura - Oued Akbou</t>
+          <t>RC Arba - GC Mascara</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>60</v>
+        <v>56.7</v>
       </c>
       <c r="F4" t="n">
         <v>1.8</v>
       </c>
       <c r="G4" t="n">
-        <v>0.08</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5">
@@ -1234,162 +1392,162 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>27-02-2025 01:30</t>
+          <t>27-02-2025 19:00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>DENMARK</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COPA DO NORDESTE</t>
+          <t>1. DIVISION</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CSA - Nautico Recife</t>
+          <t>Hvidovre - FC Fredericia</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>71.7</v>
+        <v>53.3</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.43</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>27-02-2025 19:00</t>
+          <t>27-02-2025 15:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DENMARK</t>
+          <t>EGYPT</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1. DIVISION</t>
+          <t>PREMIER LEAGUE</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hvidovre - FC Fredericia</t>
+          <t>Smouha SC - AL Masry</t>
         </is>
       </c>
       <c r="E7" t="n">
         <v>53.3</v>
       </c>
       <c r="F7" t="n">
-        <v>2.1</v>
+        <v>2.9</v>
       </c>
       <c r="G7" t="n">
-        <v>0.12</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>27-02-2025 15:00</t>
+          <t>27-02-2025 20:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EGYPT</t>
+          <t>HUNGARY</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PREMIER LEAGUE</t>
+          <t>MAGYAR KUPA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Smouha SC - AL Masry</t>
+          <t>Gyori ETO FC - Ferencvarosi TC</t>
         </is>
       </c>
       <c r="E8" t="n">
         <v>53.3</v>
       </c>
       <c r="F8" t="n">
-        <v>2.9</v>
+        <v>4</v>
       </c>
       <c r="G8" t="n">
-        <v>0.55</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>27-02-2025 20:00</t>
+          <t>27-02-2025 17:15</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HUNGARY</t>
+          <t>ICELAND</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MAGYAR KUPA</t>
+          <t>LEAGUE CUP</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Gyori ETO FC - Ferencvarosi TC</t>
+          <t>KA Akureyri - Fram Reykjavik</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>53.3</v>
+        <v>60</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>2.2</v>
       </c>
       <c r="G9" t="n">
-        <v>1.13</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>27-02-2025 17:15</t>
+          <t>27-02-2025 18:00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ICELAND</t>
+          <t>MOROCCO</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LEAGUE CUP</t>
+          <t>BOTOLA PRO</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>KA Akureyri - Fram Reykjavik</t>
+          <t>Ittihad Tanger - Riadi Salmi</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>60</v>
+        <v>57.7</v>
       </c>
       <c r="F10" t="n">
-        <v>2.2</v>
+        <v>1.77</v>
       </c>
       <c r="G10" t="n">
-        <v>0.32</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>27-02-2025 18:00</t>
+          <t>27-02-2025 20:00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1404,23 +1562,23 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Ittihad Tanger - Riadi Salmi</t>
+          <t>CODM Meknès - Hassania Agadir</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>57.7</v>
+        <v>70</v>
       </c>
       <c r="F11" t="n">
-        <v>1.77</v>
+        <v>2.05</v>
       </c>
       <c r="G11" t="n">
-        <v>0.02</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>27-02-2025 20:00</t>
+          <t>27-02-2025 22:00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1435,17 +1593,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CODM Meknès - Hassania Agadir</t>
+          <t>Difaa EL Jadida - UTS Rabat</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F12" t="n">
-        <v>2.05</v>
+        <v>2.4</v>
       </c>
       <c r="G12" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="13">
@@ -1456,120 +1614,120 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MOROCCO</t>
+          <t>PANAMA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BOTOLA PRO</t>
+          <t>LIGA PANAMEÑA DE FÚTBOL</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Difaa EL Jadida - UTS Rabat</t>
+          <t>UMECIT - Costa Del Este</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>60</v>
+        <v>53.3</v>
       </c>
       <c r="F13" t="n">
-        <v>2.4</v>
+        <v>1.95</v>
       </c>
       <c r="G13" t="n">
-        <v>0.44</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>27-02-2025 02:30</t>
+          <t>27-02-2025 18:00</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>PANAMA</t>
+          <t>POLAND</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LIGA PANAMEÑA DE FÚTBOL</t>
+          <t>CUP</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sporting San Miguelito - Veraguas</t>
+          <t>Polonia Warszawa - Puszcza Niepołomice</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F14" t="n">
-        <v>1.73</v>
+        <v>2.95</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.14</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>27-02-2025 22:00</t>
+          <t>27-02-2025 14:00</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PANAMA</t>
+          <t>SERBIA</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LIGA PANAMEÑA DE FÚTBOL</t>
+          <t>PRVA LIGA</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>UMECIT - Costa Del Este</t>
+          <t>Radnički Sr. Mitrovica - Radnik Surdulica</t>
         </is>
       </c>
       <c r="E15" t="n">
         <v>53.3</v>
       </c>
       <c r="F15" t="n">
-        <v>1.95</v>
+        <v>3</v>
       </c>
       <c r="G15" t="n">
-        <v>0.04</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>27-02-2025 18:00</t>
+          <t>27-02-2025 12:45</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>POLAND</t>
+          <t>SINGAPORE</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CUP</t>
+          <t>PREMIER LEAGUE</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Polonia Warszawa - Puszcza Niepołomice</t>
+          <t>Albirex Niigata S - Balestier Khalsa</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>70</v>
+        <v>53.3</v>
       </c>
       <c r="F16" t="n">
-        <v>2.95</v>
+        <v>2.7</v>
       </c>
       <c r="G16" t="n">
-        <v>1.06</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="17">
@@ -1580,58 +1738,58 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SERBIA</t>
+          <t>TUNISIA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PRVA LIGA</t>
+          <t>LIGUE 1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Radnički Sr. Mitrovica - Radnik Surdulica</t>
+          <t>US Tataouine - EGS Gafsa</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>53.3</v>
+        <v>66.7</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="G17" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>27-02-2025 12:45</t>
+          <t>27-02-2025 14:00</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SINGAPORE</t>
+          <t>TUNISIA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PREMIER LEAGUE</t>
+          <t>LIGUE 1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Albirex Niigata S - Balestier Khalsa</t>
+          <t>Olympique Béja - CS Sfaxien</t>
         </is>
       </c>
       <c r="E18" t="n">
         <v>53.3</v>
       </c>
       <c r="F18" t="n">
-        <v>2.7</v>
+        <v>2.25</v>
       </c>
       <c r="G18" t="n">
-        <v>0.44</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19">
@@ -1652,17 +1810,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>US Tataouine - EGS Gafsa</t>
+          <t>US Monastirienne - Club Africain</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>66.7</v>
+        <v>53.3</v>
       </c>
       <c r="F19" t="n">
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
@@ -1673,89 +1831,89 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TUNISIA</t>
+          <t>TURKEY</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>LIGUE 1</t>
+          <t>CUP</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Olympique Béja - CS Sfaxien</t>
+          <t>Kasimpasa - Goztepe</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>53.3</v>
+        <v>60</v>
       </c>
       <c r="F20" t="n">
-        <v>2.25</v>
+        <v>16</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>27-02-2025 14:25</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TUNISIA</t>
+          <t>UNITED-ARAB-EMIRATES</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LIGUE 1</t>
+          <t>DIVISION 1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>US Monastirienne - Club Africain</t>
+          <t>Hatta SC - Dubai United</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>53.3</v>
+        <v>50</v>
       </c>
       <c r="F21" t="n">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>27-02-2025 17:15</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TURKEY</t>
+          <t>UNITED-ARAB-EMIRATES</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CUP</t>
+          <t>PRO LEAGUE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Kasimpasa - Goztepe</t>
+          <t>Al Wahda FC - Al Ain</t>
         </is>
       </c>
       <c r="E22" t="n">
         <v>60</v>
       </c>
       <c r="F22" t="n">
-        <v>16</v>
+        <v>2.5</v>
       </c>
       <c r="G22" t="n">
-        <v>8.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23">
@@ -1776,48 +1934,792 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Al Wahda FC - Al Ain</t>
+          <t>Ajman - Al Nasr</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>60</v>
+        <v>53.3</v>
       </c>
       <c r="F23" t="n">
-        <v>2.5</v>
+        <v>2.64</v>
       </c>
       <c r="G23" t="n">
-        <v>0.5</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>27-02-2025 17:15</t>
+          <t>28-02-2025 20:00</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UNITED-ARAB-EMIRATES</t>
+          <t>NETHERLANDS</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PRO LEAGUE</t>
+          <t>EREDIVISIE</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Ajman - Al Nasr</t>
+          <t>Waalwijk - Fortuna Sittard</t>
         </is>
       </c>
       <c r="E24" t="n">
         <v>53.3</v>
       </c>
       <c r="F24" t="n">
-        <v>2.64</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>0.41</v>
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>28-02-2025 21:00</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SPAIN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>LA LIGA</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Valladolid - Las Palmas</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:00</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>FRANCE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>LIGUE 2</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Annecy - Paris FC</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>50</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>28-02-2025 16:00</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ROMANIA</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>LIGA I</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Unirea Slobozia - Oţelul</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>28-02-2025 01:30</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>WORLD</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>CONMEBOL LIBERTADORES</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>FBC Melgar - Deportes Tolima</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>60</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28-02-2025 01:30</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>WORLD</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>CONMEBOL RECOPA</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Botafogo - Racing Club</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>50</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>28-02-2025 19:00</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ALGERIA</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>LIGUE 1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>MC Alger - CS Constantine</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>60</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>28-02-2025 21:00</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ARGENTINA</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>PRIMERA NACIONAL</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Arsenal Sarandi - Atlanta</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>60</v>
+      </c>
+      <c r="F31" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>28-02-2025 10:15</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AUSTRALIA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>NEW SOUTH WALES NPL 2</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Blacktown Spartans - Bonnyrigg White Eagles</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>First Vienna - Stripfing</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>58</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>28-02-2025 11:00</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>AZERBAIJAN</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>BIRINCI DASTA</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Qaradağ Lökbatan - Mil-Muğan</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CYPRUS</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>1. DIVISION</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>AEL - Enosis</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>28-02-2025 15:00</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>EGYPT</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>PREMIER LEAGUE</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Ghazl El Mehalla - Enppi</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>28-02-2025 19:30</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FRANCE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>NATIONAL 1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Rouen - Concarneau</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>50</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-0.12</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>28-02-2025 19:30</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>FRANCE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>NATIONAL 1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Valenciennes - Versailles</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>60</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:30</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GERMANY</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2. BUNDESLIGA</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>FC Schalke 04 - Preußen Münster</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>50</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-0.14</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>28-02-2025 19:00</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>GERMANY</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>REGIONALLIGA - NORDOST</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>BFC Dynamo - Greifswalder FC</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:20</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>GERMANY</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>REGIONALLIGA - NORDOST</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>FSV Zwickau - Lokomotive Leipzig</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ITALY</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>SERIE C - GIRONE A</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Giana Erminio - Lumezzane</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>60</v>
+      </c>
+      <c r="F42" t="n">
+        <v>2</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>28-02-2025 22:15</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>PARAGUAY</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>DIVISION PROFESIONAL - APERTURA</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Deportivo Recoleta - Sportivo Ameliano</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>50</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>POLAND</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>EKSTRAKLASA</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Radomiak Radom - Widzew Łódź</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="F44" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>POLAND</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>I LIGA</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Pogoń Siedlce - Wisla Plock</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>50</v>
+      </c>
+      <c r="F45" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>POLAND</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>I LIGA</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Arka Gdynia - Wisla Krakow</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:30</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SOUTH-AFRICA</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PREMIER SOCCER LEAGUE</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Stellenbosch - Polokwane City</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>60</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>28-02-2025 13:15</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>VIETNAM</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>V.LEAGUE 1</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Viettel - Nam Dinh</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>60</v>
+      </c>
+      <c r="F48" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -1831,7 +2733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1879,32 +2781,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>26-02-2025 17:00</t>
+          <t>27-02-2025 14:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MALI</t>
+          <t>ALGERIA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PREMIÈRE DIVISION</t>
+          <t>LIGUE 2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>US Bougouba - Stade Malien Bamako</t>
+          <t>MB Rouisset - Usm El Harrach</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>53.3</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>2.15</v>
+        <v>3.75</v>
       </c>
       <c r="G2" t="n">
-        <v>0.15</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="3">
@@ -1941,125 +2843,342 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>27-02-2025 01:30</t>
+          <t>27-02-2025 18:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>ROMANIA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>COPA DO BRASIL</t>
+          <t>LIGA II</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Concórdia - Ponte Preta</t>
+          <t>Ceahlăul Piatra Neamţ - CSA Steaua Bucureşti</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F4" t="n">
-        <v>1.9</v>
+        <v>2.02</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.05</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>27-02-2025 22:00</t>
+          <t>27-02-2025 19:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>HONDURAS</t>
+          <t>SERBIA</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LIGA NACIONAL</t>
+          <t>SUPER LIGA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Juticalpa - Real Espana</t>
+          <t>TSC Backa Topola - Cukaricki</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>60</v>
+        <v>53.3</v>
       </c>
       <c r="F5" t="n">
-        <v>1.91</v>
+        <v>2.55</v>
       </c>
       <c r="G5" t="n">
-        <v>0.15</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>27-02-2025 18:00</t>
+          <t>28-02-2025 20:45</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ROMANIA</t>
+          <t>SCOTLAND</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LIGA II</t>
+          <t>CHAMPIONSHIP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ceahlăul Piatra Neamţ - CSA Steaua Bucureşti</t>
+          <t>Partick - Livingston</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F6" t="n">
-        <v>2.02</v>
+        <v>2.3</v>
       </c>
       <c r="G6" t="n">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>27-02-2025 19:00</t>
+          <t>28-02-2025 01:30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SERBIA</t>
+          <t>WORLD</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SUPER LIGA</t>
+          <t>CONMEBOL RECOPA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>TSC Backa Topola - Cukaricki</t>
+          <t>Botafogo - Racing Club</t>
         </is>
       </c>
       <c r="E7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>SKU Amstetten - SKN ST. Polten</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>62.3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Rapid Wien II - Austria Lustenau</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>60</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SV Horn - Voitsberg</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>60</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BELGIUM</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>JUPILER PRO LEAGUE</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Charleroi - Genk</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>53.3</v>
       </c>
-      <c r="F7" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.36</v>
+      <c r="F11" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>28-02-2025 01:30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BRAZIL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>COPA DO BRASIL</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Inter De Limeira - Vila Nova</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>60</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01-03-2025 00:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CHILE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PRIMERA DIVISIÓN</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Deportes Limache - Coquimbo Unido</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>28-02-2025 04:00</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>WORLD</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CONCACAF CHAMPIONS LEAGUE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Vancouver Whitecaps - Deportivo Saprissa</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.95</v>
       </c>
     </row>
   </sheetData>
@@ -2068,155 +3187,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Championship</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Match</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Over 2.5 (%)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Odds 2.5</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>EV over 2.5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>27-02-2025 17:00</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BULGARIA</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CUP</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Ludogorets - Botev Plovdiv</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>70</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>27-02-2025 04:05</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MEXICO</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>LIGA MX</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Atletico San Luis - Guadalajara Chivas</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>80</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>27-02-2025 14:35</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>UNITED-ARAB-EMIRATES</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>PRO LEAGUE</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Al Bataeh - Al-Ittihad Kalba</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>71.8</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2253,390 +3223,1345 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Btts (%)</t>
+          <t>Over 2.5 (%)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Odds btts</t>
+          <t>Odds 2.5</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>EV btts</t>
+          <t>EV over 2.5</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>27-02-2025 00:30</t>
+          <t>27-02-2025 17:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>BULGARIA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COPA VERDE</t>
+          <t>CUP</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Manaus FC - Paysandu</t>
+          <t>Ludogorets - Botev Plovdiv</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>81.09999999999999</v>
+        <v>70</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1.78</v>
       </c>
       <c r="G2" t="n">
-        <v>0.62</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>27-02-2025 14:35</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>UNITED-ARAB-EMIRATES</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PRO LEAGUE</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Al Bataeh - Al-Ittihad Kalba</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>71.8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Rapid Wien II - Austria Lustenau</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>85</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Ried - Floridsdorfer AC</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>85</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>First Vienna - Stripfing</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.88</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BELGIUM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>JUPILER PRO LEAGUE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Charleroi - Genk</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>70</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CYPRUS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1. DIVISION</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Anorthosis - Karmiotissa</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:20</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GERMANY</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>REGIONALLIGA - NORDOST</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FSV Zwickau - Lokomotive Leipzig</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>75</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IRELAND</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>FIRST DIVISION</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Treaty United - Finn Harps</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ITALY</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SERIE C - GIRONE A</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Giana Erminio - Lumezzane</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>75</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>28-02-2025 14:30</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>UKRAINE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PREMIER LEAGUE</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Vorskla Poltava - Dynamo Kyiv</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>70</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>28-02-2025 04:00</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>WORLD</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CONCACAF CHAMPIONS LEAGUE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Vancouver Whitecaps - Deportivo Saprissa</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Championship</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Match</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Btts (%)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Odds btts</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>EV btts</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>27-02-2025 21:00</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ENGLAND</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PREMIER LEAGUE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>West Ham - Leicester</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>27-02-2025 20:45</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ENGLAND</t>
+          <t>ITALY</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PREMIER LEAGUE</t>
+          <t>SERIE A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>West Ham - Leicester</t>
+          <t>Bologna - AC Milan</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>73.3</v>
       </c>
       <c r="F3" t="n">
-        <v>1.7</v>
+        <v>1.75</v>
       </c>
       <c r="G3" t="n">
-        <v>0.25</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>27-02-2025 20:45</t>
+          <t>27-02-2025 20:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ITALY</t>
+          <t>NETHERLANDS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SERIE A</t>
+          <t>KNVB BEKER</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bologna - AC Milan</t>
+          <t>Heracles - AZ Alkmaar</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>73.3</v>
+        <v>70</v>
       </c>
       <c r="F4" t="n">
-        <v>1.75</v>
+        <v>1.85</v>
       </c>
       <c r="G4" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>27-02-2025 20:00</t>
+          <t>27-02-2025 23:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NETHERLANDS</t>
+          <t>WORLD</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>KNVB BEKER</t>
+          <t>CONMEBOL LIBERTADORES</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Heracles - AZ Alkmaar</t>
+          <t>Cerro Porteno - Monagas SC</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="F5" t="n">
-        <v>1.85</v>
+        <v>2.1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.29</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>27-02-2025 01:30</t>
+          <t>27-02-2025 14:00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>WORLD</t>
+          <t>ALGERIA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CONMEBOL LIBERTADORES</t>
+          <t>LIGUE 2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Corinthians - UCV</t>
+          <t>JS Jijel - HB Chelghoum Laïd</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F6" t="n">
-        <v>3.5</v>
+        <v>2.3</v>
       </c>
       <c r="G6" t="n">
-        <v>1.66</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>27-02-2025 23:00</t>
+          <t>27-02-2025 17:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WORLD</t>
+          <t>BULGARIA</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CONMEBOL LIBERTADORES</t>
+          <t>CUP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Cerro Porteno - Monagas SC</t>
+          <t>Ludogorets - Botev Plovdiv</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>84</v>
+        <v>66.7</v>
       </c>
       <c r="F7" t="n">
         <v>2.1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.76</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>27-02-2025 14:00</t>
+          <t>27-02-2025 18:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ALGERIA</t>
+          <t>EGYPT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>LIGUE 2</t>
+          <t>PREMIER LEAGUE</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>JS Jijel - HB Chelghoum Laïd</t>
+          <t>Zamalek SC - Masr</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>72</v>
+        <v>76.7</v>
       </c>
       <c r="F8" t="n">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="G8" t="n">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>27-02-2025 01:00</t>
+          <t>27-02-2025 15:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BRAZIL</t>
+          <t>SERBIA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>COPA DO BRASIL</t>
+          <t>PRVA LIGA</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Humaitá - Operario-PR</t>
+          <t>Zemun - Semendrija 1924</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>84</v>
+        <v>73.3</v>
       </c>
       <c r="F9" t="n">
-        <v>2.25</v>
+        <v>2.2</v>
       </c>
       <c r="G9" t="n">
-        <v>0.89</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>27-02-2025 17:00</t>
+          <t>28-02-2025 21:00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BULGARIA</t>
+          <t>ENGLAND</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CUP</t>
+          <t>CHAMPIONSHIP</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ludogorets - Botev Plovdiv</t>
+          <t>Sheffield Wednesday - Sunderland</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>66.7</v>
+        <v>73.3</v>
       </c>
       <c r="F10" t="n">
-        <v>2.1</v>
+        <v>1.83</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>27-02-2025 18:00</t>
+          <t>28-02-2025 21:00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>EGYPT</t>
+          <t>ENGLAND</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PREMIER LEAGUE</t>
+          <t>FA CUP</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Zamalek SC - Masr</t>
+          <t>Aston Villa - Cardiff</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>76.7</v>
+        <v>88.3</v>
       </c>
       <c r="F11" t="n">
-        <v>2.15</v>
+        <v>2.1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>27-02-2025 04:05</t>
+          <t>28-02-2025 19:00</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MEXICO</t>
+          <t>DENMARK</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LIGA MX</t>
+          <t>SUPERLIGA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Atletico San Luis - Guadalajara Chivas</t>
+          <t>Randers FC - Aarhus</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F12" t="n">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>27-02-2025 15:00</t>
+          <t>28-02-2025 20:00</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SERBIA</t>
+          <t>FRANCE</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PRVA LIGA</t>
+          <t>LIGUE 2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Zemun - Semendrija 1924</t>
+          <t>Clermont Foot - Caen</t>
         </is>
       </c>
       <c r="E13" t="n">
+        <v>70</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>28-02-2025 19:30</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ITALY</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SERIE B</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Sudtirol - Spezia</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:00</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>NETHERLANDS</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>EERSTE DIVISIE</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Cambuur - VVV Venlo</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SCOTLAND</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CHAMPIONSHIP</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Partick - Livingston</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AUSTRIA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2. LIGA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>SV Lafnitz - Admira Wacker</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>73.3</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F17" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>28-02-2025 22:00</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CHILE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>PRIMERA B</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Santiago Morning - Deportes Temuco</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>01-03-2025 00:00</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CHILE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>PRIMERA DIVISIÓN</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Deportes Limache - Coquimbo Unido</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>80</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>28-02-2025 15:00</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CROATIA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>FIRST NL</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Sesvete - Rudes</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F20" t="n">
         <v>2.2</v>
       </c>
-      <c r="G13" t="n">
-        <v>0.61</v>
+      <c r="G20" t="n">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>28-02-2025 19:30</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FRANCE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NATIONAL 1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Orleans - Sochaux</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:30</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GERMANY</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2. BUNDESLIGA</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>FC Schalke 04 - Preußen Münster</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>88</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>IRELAND</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>FIRST DIVISION</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Treaty United - Finn Harps</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>IRELAND</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>PREMIER DIVISION</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Cork City - Bohemians</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:45</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>IRELAND</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>PREMIER DIVISION</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Derry City - Waterford</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>70</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ITALY</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>SERIE C - GIRONE A</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Giana Erminio - Lumezzane</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>90</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>28-02-2025 20:30</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>POLAND</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>EKSTRAKLASA</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Gornik Zabrze - Cracovia Krakow</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>70</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>28-02-2025 18:00</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>POLAND</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>I LIGA</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Pogoń Siedlce - Wisla Plock</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>68</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28-02-2025 14:30</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>UKRAINE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>PREMIER LEAGUE</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Vorskla Poltava - Dynamo Kyiv</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>28-02-2025 13:15</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>VIETNAM</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>V.LEAGUE 1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Viettel - Nam Dinh</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>